<commit_message>
silkscreen + programming connector
</commit_message>
<xml_diff>
--- a/PCB/Project Outputs for Ortho4Exent/BOM/Bill of Materials-Ortho4Exent(PRODUCTION).xlsx
+++ b/PCB/Project Outputs for Ortho4Exent/BOM/Bill of Materials-Ortho4Exent(PRODUCTION).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamasSzabo\Documents\GitHub\Ortho4Exent\PCB\Project Outputs for Ortho4Exent\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0CD0747-9C10-4889-8ABE-71A810B3DCF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1895E13D-0880-479D-A92D-8647A267AEBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" xr2:uid="{29D74E4D-55BE-4A43-B507-E09CD8F2771E}"/>
+    <workbookView xWindow="4716" yWindow="2640" windowWidth="17280" windowHeight="8964" xr2:uid="{207564E8-0610-432A-8B9F-2BADD4B8C876}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Ortho4Exent(P" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
   <si>
     <t>Designator</t>
   </si>
@@ -51,13 +51,13 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>LibRef</t>
+    <t>MANUF</t>
   </si>
   <si>
     <t>MANUFCODE</t>
   </si>
   <si>
-    <t>C1, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29</t>
+    <t>C1</t>
   </si>
   <si>
     <t>CAP SMD 0402 1 µF 10V X5R</t>
@@ -66,10 +66,34 @@
     <t>CAPC0402N</t>
   </si>
   <si>
+    <t>WE</t>
+  </si>
+  <si>
     <t>885012105012</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C6, C7, C8</t>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>CAP SMD 0805 10 µF 10 V X5R</t>
+  </si>
+  <si>
+    <t>CAPC0805N</t>
+  </si>
+  <si>
+    <t>885012107010</t>
+  </si>
+  <si>
+    <t>C3, C4</t>
+  </si>
+  <si>
+    <t>CAP SMD 0402 10 pF 10V NP0</t>
+  </si>
+  <si>
+    <t>885012005007</t>
+  </si>
+  <si>
+    <t>C5, C6, C7, C8, C9, C10, C11, C12, C13, C14, C15, C16, C17, C18, C19, C20, C21, C22, C23, C24, C25, C26, C27, C28, C29</t>
   </si>
   <si>
     <t>CAP SMD 0402 100 nF 10V X5R</t>
@@ -78,27 +102,6 @@
     <t>885012105010</t>
   </si>
   <si>
-    <t>C9</t>
-  </si>
-  <si>
-    <t>CAP SMD 0805 10 µF 10 V X5R</t>
-  </si>
-  <si>
-    <t>CAPC0805N</t>
-  </si>
-  <si>
-    <t>885012107010</t>
-  </si>
-  <si>
-    <t>C10, C11</t>
-  </si>
-  <si>
-    <t>CAP SMD 0402 10 pF 10V NP0</t>
-  </si>
-  <si>
-    <t>885012005007</t>
-  </si>
-  <si>
     <t>D1, D2, D3, D4, D5, D6, D7, D8, D9, D10, D11, D12, D13, D15, D16, D17, D18, D19, D20, D21, D22, D23, D24, D25, D26, D27, D28, D29, D30, D31, D32, D33, D34, D35, D36, D37, D38, D39, D40, D41, D42, D43, D44, D45, D46, D47, D48, D49, D50, D51, D52, D53, D54, D55, D56, D57, D58, D59, D60, D61, D62, D63, D64, D65, D66, D67, D68, D69, D70, D71</t>
   </si>
   <si>
@@ -108,6 +111,9 @@
     <t>SOD323FL</t>
   </si>
   <si>
+    <t>ON Semi</t>
+  </si>
+  <si>
     <t>1N4148WT</t>
   </si>
   <si>
@@ -120,6 +126,9 @@
     <t>513870530</t>
   </si>
   <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
     <t>LED1, LED2, LED3, LED4, LED5, LED6, LED7, LED8, LED9, LED10, LED11, LED12, LED13, LED14, LED15, LED16, LED17, LED18</t>
   </si>
   <si>
@@ -129,10 +138,13 @@
     <t>WS2812</t>
   </si>
   <si>
+    <t>Worldsemi</t>
+  </si>
+  <si>
     <t>WS2812B</t>
   </si>
   <si>
-    <t>R1, R4</t>
+    <t>R1, R2</t>
   </si>
   <si>
     <t>RES SMD 22 OHM 1% 1/10W 100PPM 0603</t>
@@ -141,10 +153,13 @@
     <t>RESC0603N</t>
   </si>
   <si>
+    <t>VISHAY</t>
+  </si>
+  <si>
     <t>CRCW060322R0FKEA</t>
   </si>
   <si>
-    <t>R5, R6</t>
+    <t>R3, R4</t>
   </si>
   <si>
     <t>RES SMD 4.7K OHM 1% 1/16W 100PPM 0402</t>
@@ -165,22 +180,34 @@
     <t>434153017835</t>
   </si>
   <si>
-    <t xml:space="preserve">434153017835 </t>
-  </si>
-  <si>
-    <t>U1, Y1</t>
-  </si>
-  <si>
-    <t>IC MCU 8BIT 32KB FLASH 44VQFN, CRYSTAL 16.0000MHZ 18PF SMD</t>
-  </si>
-  <si>
-    <t>44PW_M, WE-XTAL_CFPX-180</t>
-  </si>
-  <si>
-    <t>CMP-0095-00166-2, 830055951</t>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>IC MCU 8BIT 32KB FLASH 44VQFN</t>
+  </si>
+  <si>
+    <t>44PW_M</t>
+  </si>
+  <si>
+    <t>Microchip</t>
   </si>
   <si>
     <t>ATMEGA32U4-MU-ND</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>CRYSTAL 16.0000MHZ 18PF SMD</t>
+  </si>
+  <si>
+    <t>WE-XTAL_CFPX-180</t>
+  </si>
+  <si>
+    <t>WE/IQD</t>
+  </si>
+  <si>
+    <t>830055951</t>
   </si>
 </sst>
 </file>
@@ -562,20 +589,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98257D7-2869-41B2-A041-864BB5DF7419}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A76D567-2A12-45F3-B7F6-4D4E903C70B1}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="3" max="3" width="35" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -598,12 +625,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -615,212 +642,232 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4">
         <v>70</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4">
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B9" s="4">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B11" s="4">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="69" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
+  <pageSetup scale="88" orientation="landscape" blackAndWhite="1" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
V1 . do not order, see change list
Change list for version 2:
1. USB pinout
2. WS2812 silkscreen
3. BOM on silkscreen
4. Diode order code
</commit_message>
<xml_diff>
--- a/PCB/Project Outputs for Ortho4Exent/BOM/Bill of Materials-Ortho4Exent(PRODUCTION).xlsx
+++ b/PCB/Project Outputs for Ortho4Exent/BOM/Bill of Materials-Ortho4Exent(PRODUCTION).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TamasSzabo\Documents\GitHub\Ortho4Exent\PCB\Project Outputs for Ortho4Exent\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41EA4B9B-657A-41AF-B595-BB072EA6D95C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{23C73A7E-DDD0-4632-9F94-7DAFA81190A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4716" yWindow="2640" windowWidth="17280" windowHeight="8964" xr2:uid="{2A1DA2BE-C072-46EF-B342-F3D5CEB99D0C}"/>
+    <workbookView xWindow="23808" yWindow="-3396" windowWidth="23040" windowHeight="12204" xr2:uid="{A7FE20A5-6398-47F6-ACFE-9831F8BF0DC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Ortho4Exent(P" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Designator</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>D72</t>
+  </si>
+  <si>
+    <t>WE-TVS TVS Diode, High Speed Series, SOT23-6L, VDC = 5V</t>
   </si>
   <si>
     <t>SOT23-6L</t>
@@ -595,7 +598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA125010-5F16-475A-96B7-EB0A1ED61BFD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE827FF5-6D89-4C67-BC25-094828340C5C}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -731,163 +734,165 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="D7" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" s="4">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4">
         <v>2</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B11" s="4">
         <v>2</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4">
         <v>1</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="4">
         <v>1</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B14" s="4">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup scale="86" orientation="landscape" blackAndWhite="1" verticalDpi="0" r:id="rId1"/>
+  <pageSetup scale="84" orientation="landscape" blackAndWhite="1" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>